<commit_message>
update GenChartByAi 7 (gpt-3.5-turbo)
</commit_message>
<xml_diff>
--- a/doc/Excel/Book1.xlsx
+++ b/doc/Excel/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Self learn\kokshengbi\kokshengbi-backend\doc\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9294D459-FC3C-4AE0-B93D-751397CF09D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FE8123-5938-4946-BAA2-41821829197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE428E32-D580-4ADD-84A3-47DC43BDA153}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="22605" windowHeight="13680" xr2:uid="{DE428E32-D580-4ADD-84A3-47DC43BDA153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -449,7 +449,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>